<commit_message>
Update with Hidden Spring
</commit_message>
<xml_diff>
--- a/File Library/Source Files/Chrisousel/BOM.xlsx
+++ b/File Library/Source Files/Chrisousel/BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>BOM for Chrisousel</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>0.7 Wire Diameter, 8mm OD, 15mm Height</t>
+  </si>
+  <si>
+    <t>MR115 Bearings</t>
+  </si>
+  <si>
+    <t>Likely to be replaced</t>
   </si>
 </sst>
 </file>
@@ -426,7 +432,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
@@ -560,12 +566,23 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>19</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>1</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>